<commit_message>
Cambios de evaluacion Base por escritura de tesis
</commit_message>
<xml_diff>
--- a/02_BASE/modelo_base_VAN.xlsx
+++ b/02_BASE/modelo_base_VAN.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documentos\(Proyecto)_Estudio_PKPD\VANCOMICINA\02_BASE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7605" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="modelos_base" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="123">
   <si>
     <t>Project Name</t>
   </si>
@@ -365,6 +365,36 @@
   </si>
   <si>
     <t>Logarítmo</t>
+  </si>
+  <si>
+    <t>Select for reference</t>
+  </si>
+  <si>
+    <t>nbexploratoryiterations</t>
+  </si>
+  <si>
+    <t>nbsmoothingiterations</t>
+  </si>
+  <si>
+    <t>Maximum number of iterations</t>
+  </si>
+  <si>
+    <t>Minimum number of iterations (miniterations)</t>
+  </si>
+  <si>
+    <t>Prueba de Chi Cuadrado</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Comparativo 1CPTM vs 2CPTM</t>
+  </si>
+  <si>
+    <t>LRT</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Comparativo 2CPTM vs 3CPTM</t>
   </si>
 </sst>
 </file>
@@ -374,7 +404,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -438,6 +468,39 @@
       <color rgb="FFFF0000"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -631,7 +694,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -831,81 +894,159 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1186,13 +1327,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:S95"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="A24" sqref="A24:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -1358,15 +1500,15 @@
       <c r="A6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="91"/>
-      <c r="C6" s="91"/>
-      <c r="D6" s="91"/>
-      <c r="E6" s="91"/>
-      <c r="F6" s="91"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="91"/>
-      <c r="I6" s="91"/>
-      <c r="J6" s="93"/>
+      <c r="B6" s="86"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="88"/>
       <c r="K6"/>
       <c r="L6"/>
       <c r="M6"/>
@@ -1381,15 +1523,15 @@
       <c r="A7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="92"/>
-      <c r="C7" s="92"/>
-      <c r="D7" s="92"/>
-      <c r="E7" s="92"/>
-      <c r="F7" s="92"/>
-      <c r="G7" s="92"/>
-      <c r="H7" s="92"/>
-      <c r="I7" s="92"/>
-      <c r="J7" s="94"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="87"/>
+      <c r="D7" s="87"/>
+      <c r="E7" s="87"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="87"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="89"/>
       <c r="K7" s="18"/>
       <c r="L7" s="18"/>
       <c r="M7" s="18"/>
@@ -1593,7 +1735,7 @@
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19" ht="15">
-      <c r="A14" s="70" t="s">
+      <c r="A14" s="84" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="50">
@@ -1605,12 +1747,12 @@
       <c r="D14" s="50">
         <v>54.62</v>
       </c>
-      <c r="E14" s="83"/>
-      <c r="F14" s="83"/>
-      <c r="G14" s="83"/>
-      <c r="H14" s="83"/>
-      <c r="I14" s="83"/>
-      <c r="J14" s="89"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="80"/>
+      <c r="J14" s="82"/>
       <c r="K14"/>
       <c r="L14"/>
       <c r="M14"/>
@@ -1622,7 +1764,7 @@
       <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A15" s="72"/>
+      <c r="A15" s="85"/>
       <c r="B15" s="51">
         <v>2.5199999999999998E-7</v>
       </c>
@@ -1632,12 +1774,12 @@
       <c r="D15" s="51">
         <v>5.5500000000000001E-2</v>
       </c>
-      <c r="E15" s="84"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="84"/>
-      <c r="H15" s="84"/>
-      <c r="I15" s="84"/>
-      <c r="J15" s="90"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="81"/>
+      <c r="G15" s="81"/>
+      <c r="H15" s="81"/>
+      <c r="I15" s="81"/>
+      <c r="J15" s="83"/>
       <c r="K15"/>
       <c r="L15"/>
       <c r="M15"/>
@@ -1649,7 +1791,7 @@
       <c r="S15" s="1"/>
     </row>
     <row r="16" spans="1:19" ht="15">
-      <c r="A16" s="70" t="s">
+      <c r="A16" s="84" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="52">
@@ -1690,7 +1832,7 @@
       <c r="S16" s="1"/>
     </row>
     <row r="17" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A17" s="72"/>
+      <c r="A17" s="85"/>
       <c r="B17" s="54">
         <v>6.7699999999999996E-2</v>
       </c>
@@ -1729,21 +1871,21 @@
       <c r="S17" s="1"/>
     </row>
     <row r="18" spans="1:19" ht="15">
-      <c r="A18" s="70" t="s">
+      <c r="A18" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="83"/>
-      <c r="C18" s="83"/>
+      <c r="B18" s="80"/>
+      <c r="C18" s="80"/>
       <c r="D18" s="50">
         <v>0.90800000000000003</v>
       </c>
-      <c r="E18" s="83"/>
-      <c r="F18" s="83"/>
+      <c r="E18" s="80"/>
+      <c r="F18" s="80"/>
       <c r="G18" s="50">
         <v>0.91100000000000003</v>
       </c>
-      <c r="H18" s="83"/>
-      <c r="I18" s="83"/>
+      <c r="H18" s="80"/>
+      <c r="I18" s="80"/>
       <c r="J18" s="56">
         <v>0.91200000000000003</v>
       </c>
@@ -1758,19 +1900,19 @@
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A19" s="72"/>
-      <c r="B19" s="84"/>
-      <c r="C19" s="84"/>
+      <c r="A19" s="85"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="81"/>
       <c r="D19" s="51">
         <v>5.8299999999999998E-2</v>
       </c>
-      <c r="E19" s="84"/>
-      <c r="F19" s="84"/>
+      <c r="E19" s="81"/>
+      <c r="F19" s="81"/>
       <c r="G19" s="51">
         <v>5.96E-2</v>
       </c>
-      <c r="H19" s="84"/>
-      <c r="I19" s="84"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="81"/>
       <c r="J19" s="57">
         <v>5.9499999999999997E-2</v>
       </c>
@@ -1785,12 +1927,12 @@
       <c r="S19" s="1"/>
     </row>
     <row r="20" spans="1:19" ht="15">
-      <c r="A20" s="70" t="s">
+      <c r="A20" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="87"/>
-      <c r="C20" s="87"/>
-      <c r="D20" s="87"/>
+      <c r="B20" s="90"/>
+      <c r="C20" s="90"/>
+      <c r="D20" s="90"/>
       <c r="E20" s="52">
         <v>53.69</v>
       </c>
@@ -1820,10 +1962,10 @@
       <c r="S20" s="1"/>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A21" s="72"/>
-      <c r="B21" s="88"/>
-      <c r="C21" s="88"/>
-      <c r="D21" s="88"/>
+      <c r="A21" s="85"/>
+      <c r="B21" s="91"/>
+      <c r="C21" s="91"/>
+      <c r="D21" s="91"/>
       <c r="E21" s="54">
         <v>3.3099999999999999E-7</v>
       </c>
@@ -1853,12 +1995,12 @@
       <c r="S21" s="1"/>
     </row>
     <row r="22" spans="1:19" ht="15">
-      <c r="A22" s="70" t="s">
+      <c r="A22" s="84" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="83"/>
-      <c r="C22" s="83"/>
-      <c r="D22" s="83"/>
+      <c r="B22" s="80"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
       <c r="E22" s="50">
         <v>15.97</v>
       </c>
@@ -1868,9 +2010,9 @@
       <c r="G22" s="50">
         <v>14.14</v>
       </c>
-      <c r="H22" s="83"/>
-      <c r="I22" s="83"/>
-      <c r="J22" s="89"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="80"/>
+      <c r="J22" s="82"/>
       <c r="K22"/>
       <c r="L22"/>
       <c r="M22"/>
@@ -1882,10 +2024,10 @@
       <c r="S22" s="1"/>
     </row>
     <row r="23" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A23" s="72"/>
-      <c r="B23" s="84"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
+      <c r="A23" s="85"/>
+      <c r="B23" s="81"/>
+      <c r="C23" s="81"/>
+      <c r="D23" s="81"/>
       <c r="E23" s="51">
         <v>1.1600000000000001E-7</v>
       </c>
@@ -1895,9 +2037,9 @@
       <c r="G23" s="51">
         <v>5.6700000000000003E-7</v>
       </c>
-      <c r="H23" s="84"/>
-      <c r="I23" s="84"/>
-      <c r="J23" s="90"/>
+      <c r="H23" s="81"/>
+      <c r="I23" s="81"/>
+      <c r="J23" s="83"/>
       <c r="K23"/>
       <c r="L23"/>
       <c r="M23"/>
@@ -1909,12 +2051,12 @@
       <c r="S23" s="1"/>
     </row>
     <row r="24" spans="1:19" ht="15">
-      <c r="A24" s="70" t="s">
+      <c r="A24" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="87"/>
-      <c r="C24" s="87"/>
-      <c r="D24" s="87"/>
+      <c r="B24" s="90"/>
+      <c r="C24" s="90"/>
+      <c r="D24" s="90"/>
       <c r="E24" s="52">
         <v>44.1</v>
       </c>
@@ -1944,10 +2086,10 @@
       <c r="S24" s="1"/>
     </row>
     <row r="25" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A25" s="72"/>
-      <c r="B25" s="88"/>
-      <c r="C25" s="88"/>
-      <c r="D25" s="88"/>
+      <c r="A25" s="85"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="91"/>
+      <c r="D25" s="91"/>
       <c r="E25" s="58">
         <v>1.2684</v>
       </c>
@@ -1977,16 +2119,16 @@
       <c r="S25" s="1"/>
     </row>
     <row r="26" spans="1:19" ht="15">
-      <c r="A26" s="70" t="s">
+      <c r="A26" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="83"/>
-      <c r="C26" s="83"/>
-      <c r="D26" s="83"/>
-      <c r="E26" s="83"/>
-      <c r="F26" s="83"/>
-      <c r="G26" s="83"/>
-      <c r="H26" s="85">
+      <c r="B26" s="80"/>
+      <c r="C26" s="80"/>
+      <c r="D26" s="80"/>
+      <c r="E26" s="80"/>
+      <c r="F26" s="80"/>
+      <c r="G26" s="80"/>
+      <c r="H26" s="92">
         <v>12.78</v>
       </c>
       <c r="I26" s="50">
@@ -2006,14 +2148,14 @@
       <c r="S26" s="1"/>
     </row>
     <row r="27" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A27" s="72"/>
-      <c r="B27" s="84"/>
-      <c r="C27" s="84"/>
-      <c r="D27" s="84"/>
-      <c r="E27" s="84"/>
-      <c r="F27" s="84"/>
-      <c r="G27" s="84"/>
-      <c r="H27" s="86"/>
+      <c r="A27" s="85"/>
+      <c r="B27" s="81"/>
+      <c r="C27" s="81"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="81"/>
+      <c r="G27" s="81"/>
+      <c r="H27" s="93"/>
       <c r="I27" s="51">
         <v>0.33610000000000001</v>
       </c>
@@ -2031,15 +2173,15 @@
       <c r="S27" s="1"/>
     </row>
     <row r="28" spans="1:19" ht="15">
-      <c r="A28" s="70" t="s">
+      <c r="A28" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="87"/>
-      <c r="C28" s="87"/>
-      <c r="D28" s="87"/>
-      <c r="E28" s="87"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87"/>
+      <c r="B28" s="90"/>
+      <c r="C28" s="90"/>
+      <c r="D28" s="90"/>
+      <c r="E28" s="90"/>
+      <c r="F28" s="90"/>
+      <c r="G28" s="90"/>
       <c r="H28" s="52">
         <v>0.29799999999999999</v>
       </c>
@@ -2060,13 +2202,13 @@
       <c r="S28" s="1"/>
     </row>
     <row r="29" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A29" s="72"/>
-      <c r="B29" s="88"/>
-      <c r="C29" s="88"/>
-      <c r="D29" s="88"/>
-      <c r="E29" s="88"/>
-      <c r="F29" s="88"/>
-      <c r="G29" s="88"/>
+      <c r="A29" s="85"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="91"/>
+      <c r="D29" s="91"/>
+      <c r="E29" s="91"/>
+      <c r="F29" s="91"/>
+      <c r="G29" s="91"/>
       <c r="H29" s="54">
         <v>2.2399999999999999E-8</v>
       </c>
@@ -2087,15 +2229,15 @@
       <c r="S29" s="1"/>
     </row>
     <row r="30" spans="1:19" ht="15">
-      <c r="A30" s="70" t="s">
+      <c r="A30" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="83"/>
-      <c r="C30" s="83"/>
-      <c r="D30" s="83"/>
-      <c r="E30" s="83"/>
-      <c r="F30" s="83"/>
-      <c r="G30" s="83"/>
+      <c r="B30" s="80"/>
+      <c r="C30" s="80"/>
+      <c r="D30" s="80"/>
+      <c r="E30" s="80"/>
+      <c r="F30" s="80"/>
+      <c r="G30" s="80"/>
       <c r="H30" s="50">
         <v>0.52600000000000002</v>
       </c>
@@ -2116,13 +2258,13 @@
       <c r="S30" s="1"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A31" s="72"/>
-      <c r="B31" s="84"/>
-      <c r="C31" s="84"/>
-      <c r="D31" s="84"/>
-      <c r="E31" s="84"/>
-      <c r="F31" s="84"/>
-      <c r="G31" s="84"/>
+      <c r="A31" s="85"/>
+      <c r="B31" s="81"/>
+      <c r="C31" s="81"/>
+      <c r="D31" s="81"/>
+      <c r="E31" s="81"/>
+      <c r="F31" s="81"/>
+      <c r="G31" s="81"/>
       <c r="H31" s="51">
         <v>9.83E-8</v>
       </c>
@@ -2184,7 +2326,7 @@
       <c r="S32" s="1"/>
     </row>
     <row r="33" spans="1:19" ht="15">
-      <c r="A33" s="70" t="s">
+      <c r="A33" s="84" t="s">
         <v>42</v>
       </c>
       <c r="B33" s="31">
@@ -2225,7 +2367,7 @@
       <c r="S33" s="1"/>
     </row>
     <row r="34" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A34" s="72"/>
+      <c r="A34" s="85"/>
       <c r="B34" s="32">
         <v>0.21129999999999999</v>
       </c>
@@ -2264,7 +2406,7 @@
       <c r="S34" s="1"/>
     </row>
     <row r="35" spans="1:19" ht="15">
-      <c r="A35" s="70" t="s">
+      <c r="A35" s="84" t="s">
         <v>43</v>
       </c>
       <c r="B35" s="34">
@@ -2276,12 +2418,12 @@
       <c r="D35" s="34">
         <v>0.16500000000000001</v>
       </c>
-      <c r="E35" s="73"/>
-      <c r="F35" s="73"/>
-      <c r="G35" s="73"/>
-      <c r="H35" s="73"/>
-      <c r="I35" s="73"/>
-      <c r="J35" s="81"/>
+      <c r="E35" s="98"/>
+      <c r="F35" s="98"/>
+      <c r="G35" s="98"/>
+      <c r="H35" s="98"/>
+      <c r="I35" s="98"/>
+      <c r="J35" s="94"/>
       <c r="K35"/>
       <c r="L35"/>
       <c r="M35"/>
@@ -2293,7 +2435,7 @@
       <c r="S35" s="1"/>
     </row>
     <row r="36" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A36" s="72"/>
+      <c r="A36" s="85"/>
       <c r="B36" s="59">
         <v>0.75949999999999995</v>
       </c>
@@ -2303,12 +2445,12 @@
       <c r="D36" s="35">
         <v>0.32319999999999999</v>
       </c>
-      <c r="E36" s="74"/>
-      <c r="F36" s="74"/>
-      <c r="G36" s="74"/>
-      <c r="H36" s="74"/>
-      <c r="I36" s="74"/>
-      <c r="J36" s="82"/>
+      <c r="E36" s="99"/>
+      <c r="F36" s="99"/>
+      <c r="G36" s="99"/>
+      <c r="H36" s="99"/>
+      <c r="I36" s="99"/>
+      <c r="J36" s="95"/>
       <c r="K36"/>
       <c r="L36"/>
       <c r="M36"/>
@@ -2320,21 +2462,21 @@
       <c r="S36" s="1"/>
     </row>
     <row r="37" spans="1:19" ht="15">
-      <c r="A37" s="70" t="s">
+      <c r="A37" s="84" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="68"/>
-      <c r="C37" s="68"/>
+      <c r="B37" s="96"/>
+      <c r="C37" s="96"/>
       <c r="D37" s="31">
         <v>0.192</v>
       </c>
-      <c r="E37" s="68"/>
-      <c r="F37" s="68"/>
+      <c r="E37" s="96"/>
+      <c r="F37" s="96"/>
       <c r="G37" s="31">
         <v>0.21</v>
       </c>
-      <c r="H37" s="68"/>
-      <c r="I37" s="68"/>
+      <c r="H37" s="96"/>
+      <c r="I37" s="96"/>
       <c r="J37" s="37">
         <v>0.21</v>
       </c>
@@ -2349,19 +2491,19 @@
       <c r="S37" s="1"/>
     </row>
     <row r="38" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A38" s="72"/>
-      <c r="B38" s="69"/>
-      <c r="C38" s="69"/>
+      <c r="A38" s="85"/>
+      <c r="B38" s="97"/>
+      <c r="C38" s="97"/>
       <c r="D38" s="32">
         <v>0.2281</v>
       </c>
-      <c r="E38" s="69"/>
-      <c r="F38" s="69"/>
+      <c r="E38" s="97"/>
+      <c r="F38" s="97"/>
       <c r="G38" s="32">
         <v>0.20580000000000001</v>
       </c>
-      <c r="H38" s="69"/>
-      <c r="I38" s="69"/>
+      <c r="H38" s="97"/>
+      <c r="I38" s="97"/>
       <c r="J38" s="30">
         <v>0.20169999999999999</v>
       </c>
@@ -2376,12 +2518,12 @@
       <c r="S38" s="1"/>
     </row>
     <row r="39" spans="1:19" ht="15">
-      <c r="A39" s="70" t="s">
+      <c r="A39" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="73"/>
-      <c r="C39" s="73"/>
-      <c r="D39" s="73"/>
+      <c r="B39" s="98"/>
+      <c r="C39" s="98"/>
+      <c r="D39" s="98"/>
       <c r="E39" s="34">
         <v>3.4200000000000002E-8</v>
       </c>
@@ -2391,9 +2533,9 @@
       <c r="G39" s="34">
         <v>5.4900000000000002E-8</v>
       </c>
-      <c r="H39" s="73"/>
-      <c r="I39" s="73"/>
-      <c r="J39" s="81"/>
+      <c r="H39" s="98"/>
+      <c r="I39" s="98"/>
+      <c r="J39" s="94"/>
       <c r="K39"/>
       <c r="L39"/>
       <c r="M39"/>
@@ -2405,10 +2547,10 @@
       <c r="S39" s="1"/>
     </row>
     <row r="40" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A40" s="72"/>
-      <c r="B40" s="74"/>
-      <c r="C40" s="74"/>
-      <c r="D40" s="74"/>
+      <c r="A40" s="85"/>
+      <c r="B40" s="99"/>
+      <c r="C40" s="99"/>
+      <c r="D40" s="99"/>
       <c r="E40" s="59">
         <v>1.5450999999999999</v>
       </c>
@@ -2418,9 +2560,9 @@
       <c r="G40" s="59">
         <v>0.97760000000000002</v>
       </c>
-      <c r="H40" s="74"/>
-      <c r="I40" s="74"/>
-      <c r="J40" s="82"/>
+      <c r="H40" s="99"/>
+      <c r="I40" s="99"/>
+      <c r="J40" s="95"/>
       <c r="K40"/>
       <c r="L40"/>
       <c r="M40"/>
@@ -2432,12 +2574,12 @@
       <c r="S40" s="1"/>
     </row>
     <row r="41" spans="1:19" ht="15">
-      <c r="A41" s="70" t="s">
+      <c r="A41" s="84" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="68"/>
-      <c r="C41" s="68"/>
-      <c r="D41" s="68"/>
+      <c r="B41" s="96"/>
+      <c r="C41" s="96"/>
+      <c r="D41" s="96"/>
       <c r="E41" s="31">
         <v>5.39E-8</v>
       </c>
@@ -2467,10 +2609,10 @@
       <c r="S41" s="1"/>
     </row>
     <row r="42" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A42" s="72"/>
-      <c r="B42" s="69"/>
-      <c r="C42" s="69"/>
-      <c r="D42" s="69"/>
+      <c r="A42" s="85"/>
+      <c r="B42" s="97"/>
+      <c r="C42" s="97"/>
+      <c r="D42" s="97"/>
       <c r="E42" s="60">
         <v>1.1594</v>
       </c>
@@ -2500,12 +2642,12 @@
       <c r="S42" s="1"/>
     </row>
     <row r="43" spans="1:19" ht="15">
-      <c r="A43" s="70" t="s">
+      <c r="A43" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="73"/>
-      <c r="C43" s="73"/>
-      <c r="D43" s="73"/>
+      <c r="B43" s="98"/>
+      <c r="C43" s="98"/>
+      <c r="D43" s="98"/>
       <c r="E43" s="34">
         <v>0.99299999999999999</v>
       </c>
@@ -2518,7 +2660,7 @@
       <c r="H43" s="34">
         <v>1.1399999999999999</v>
       </c>
-      <c r="I43" s="79">
+      <c r="I43" s="100">
         <v>2.0100000000000001E-8</v>
       </c>
       <c r="J43" s="36">
@@ -2535,10 +2677,10 @@
       <c r="S43" s="1"/>
     </row>
     <row r="44" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A44" s="72"/>
-      <c r="B44" s="74"/>
-      <c r="C44" s="74"/>
-      <c r="D44" s="74"/>
+      <c r="A44" s="85"/>
+      <c r="B44" s="99"/>
+      <c r="C44" s="99"/>
+      <c r="D44" s="99"/>
       <c r="E44" s="59">
         <v>1.0032000000000001</v>
       </c>
@@ -2551,7 +2693,7 @@
       <c r="H44" s="59">
         <v>0.66069999999999995</v>
       </c>
-      <c r="I44" s="80"/>
+      <c r="I44" s="101"/>
       <c r="J44" s="33">
         <v>0.58809999999999996</v>
       </c>
@@ -2566,22 +2708,22 @@
       <c r="S44" s="1"/>
     </row>
     <row r="45" spans="1:19" ht="15">
-      <c r="A45" s="70" t="s">
+      <c r="A45" s="84" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="68"/>
-      <c r="C45" s="68"/>
-      <c r="D45" s="68"/>
-      <c r="E45" s="68"/>
-      <c r="F45" s="68"/>
-      <c r="G45" s="68"/>
+      <c r="B45" s="96"/>
+      <c r="C45" s="96"/>
+      <c r="D45" s="96"/>
+      <c r="E45" s="96"/>
+      <c r="F45" s="96"/>
+      <c r="G45" s="96"/>
       <c r="H45" s="31">
         <v>2.6799999999999998E-8</v>
       </c>
       <c r="I45" s="31">
         <v>1.04</v>
       </c>
-      <c r="J45" s="77">
+      <c r="J45" s="102">
         <v>3.77E-8</v>
       </c>
       <c r="K45"/>
@@ -2595,20 +2737,20 @@
       <c r="S45" s="1"/>
     </row>
     <row r="46" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A46" s="72"/>
-      <c r="B46" s="69"/>
-      <c r="C46" s="69"/>
-      <c r="D46" s="69"/>
-      <c r="E46" s="69"/>
-      <c r="F46" s="69"/>
-      <c r="G46" s="69"/>
+      <c r="A46" s="85"/>
+      <c r="B46" s="97"/>
+      <c r="C46" s="97"/>
+      <c r="D46" s="97"/>
+      <c r="E46" s="97"/>
+      <c r="F46" s="97"/>
+      <c r="G46" s="97"/>
       <c r="H46" s="60">
         <v>1.5006999999999999</v>
       </c>
       <c r="I46" s="32">
         <v>0.33750000000000002</v>
       </c>
-      <c r="J46" s="78"/>
+      <c r="J46" s="103"/>
       <c r="K46"/>
       <c r="L46"/>
       <c r="M46"/>
@@ -2620,15 +2762,15 @@
       <c r="S46" s="1"/>
     </row>
     <row r="47" spans="1:19" ht="15">
-      <c r="A47" s="70" t="s">
+      <c r="A47" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="B47" s="73"/>
-      <c r="C47" s="73"/>
-      <c r="D47" s="73"/>
-      <c r="E47" s="73"/>
-      <c r="F47" s="73"/>
-      <c r="G47" s="73"/>
+      <c r="B47" s="98"/>
+      <c r="C47" s="98"/>
+      <c r="D47" s="98"/>
+      <c r="E47" s="98"/>
+      <c r="F47" s="98"/>
+      <c r="G47" s="98"/>
       <c r="H47" s="34">
         <v>1.6400000000000001E-8</v>
       </c>
@@ -2649,13 +2791,13 @@
       <c r="S47" s="1"/>
     </row>
     <row r="48" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A48" s="72"/>
-      <c r="B48" s="74"/>
-      <c r="C48" s="74"/>
-      <c r="D48" s="74"/>
-      <c r="E48" s="74"/>
-      <c r="F48" s="74"/>
-      <c r="G48" s="74"/>
+      <c r="A48" s="85"/>
+      <c r="B48" s="99"/>
+      <c r="C48" s="99"/>
+      <c r="D48" s="99"/>
+      <c r="E48" s="99"/>
+      <c r="F48" s="99"/>
+      <c r="G48" s="99"/>
       <c r="H48" s="59">
         <v>1.6798</v>
       </c>
@@ -2676,15 +2818,15 @@
       <c r="S48" s="1"/>
     </row>
     <row r="49" spans="1:19" ht="15">
-      <c r="A49" s="70" t="s">
+      <c r="A49" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="B49" s="68"/>
-      <c r="C49" s="68"/>
-      <c r="D49" s="68"/>
-      <c r="E49" s="68"/>
-      <c r="F49" s="68"/>
-      <c r="G49" s="68"/>
+      <c r="B49" s="96"/>
+      <c r="C49" s="96"/>
+      <c r="D49" s="96"/>
+      <c r="E49" s="96"/>
+      <c r="F49" s="96"/>
+      <c r="G49" s="96"/>
       <c r="H49" s="31">
         <v>5.39E-8</v>
       </c>
@@ -2705,13 +2847,13 @@
       <c r="S49" s="1"/>
     </row>
     <row r="50" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A50" s="72"/>
-      <c r="B50" s="69"/>
-      <c r="C50" s="69"/>
-      <c r="D50" s="69"/>
-      <c r="E50" s="69"/>
-      <c r="F50" s="69"/>
-      <c r="G50" s="69"/>
+      <c r="A50" s="85"/>
+      <c r="B50" s="97"/>
+      <c r="C50" s="97"/>
+      <c r="D50" s="97"/>
+      <c r="E50" s="97"/>
+      <c r="F50" s="97"/>
+      <c r="G50" s="97"/>
       <c r="H50" s="60">
         <v>1.1082000000000001</v>
       </c>
@@ -2773,7 +2915,7 @@
       <c r="S51" s="1"/>
     </row>
     <row r="52" spans="1:19" ht="15">
-      <c r="A52" s="70" t="s">
+      <c r="A52" s="84" t="s">
         <v>52</v>
       </c>
       <c r="B52" s="31">
@@ -2782,21 +2924,21 @@
       <c r="C52" s="31">
         <v>3.34</v>
       </c>
-      <c r="D52" s="68"/>
+      <c r="D52" s="96"/>
       <c r="E52" s="31">
         <v>2.2799999999999998</v>
       </c>
       <c r="F52" s="31">
         <v>1.79</v>
       </c>
-      <c r="G52" s="68"/>
+      <c r="G52" s="96"/>
       <c r="H52" s="31">
         <v>2.3199999999999998</v>
       </c>
       <c r="I52" s="31">
         <v>1.78</v>
       </c>
-      <c r="J52" s="75"/>
+      <c r="J52" s="104"/>
       <c r="K52"/>
       <c r="L52"/>
       <c r="M52"/>
@@ -2808,28 +2950,28 @@
       <c r="S52" s="1"/>
     </row>
     <row r="53" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A53" s="72"/>
+      <c r="A53" s="85"/>
       <c r="B53" s="32">
         <v>7.7700000000000005E-2</v>
       </c>
       <c r="C53" s="32">
         <v>8.48E-2</v>
       </c>
-      <c r="D53" s="69"/>
+      <c r="D53" s="97"/>
       <c r="E53" s="32">
         <v>8.48E-2</v>
       </c>
       <c r="F53" s="32">
         <v>9.3899999999999997E-2</v>
       </c>
-      <c r="G53" s="69"/>
+      <c r="G53" s="97"/>
       <c r="H53" s="32">
         <v>8.7400000000000005E-2</v>
       </c>
       <c r="I53" s="32">
         <v>0.106</v>
       </c>
-      <c r="J53" s="76"/>
+      <c r="J53" s="105"/>
       <c r="K53"/>
       <c r="L53"/>
       <c r="M53"/>
@@ -2841,21 +2983,21 @@
       <c r="S53" s="1"/>
     </row>
     <row r="54" spans="1:19" ht="15">
-      <c r="A54" s="70" t="s">
+      <c r="A54" s="84" t="s">
         <v>53</v>
       </c>
-      <c r="B54" s="73"/>
-      <c r="C54" s="73"/>
+      <c r="B54" s="98"/>
+      <c r="C54" s="98"/>
       <c r="D54" s="34">
         <v>3.44</v>
       </c>
-      <c r="E54" s="73"/>
-      <c r="F54" s="73"/>
+      <c r="E54" s="98"/>
+      <c r="F54" s="98"/>
       <c r="G54" s="34">
         <v>1.97</v>
       </c>
-      <c r="H54" s="73"/>
-      <c r="I54" s="73"/>
+      <c r="H54" s="98"/>
+      <c r="I54" s="98"/>
       <c r="J54" s="36">
         <v>1.96</v>
       </c>
@@ -2870,19 +3012,19 @@
       <c r="S54" s="1"/>
     </row>
     <row r="55" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A55" s="72"/>
-      <c r="B55" s="74"/>
-      <c r="C55" s="74"/>
+      <c r="A55" s="85"/>
+      <c r="B55" s="99"/>
+      <c r="C55" s="99"/>
       <c r="D55" s="35">
         <v>8.4699999999999998E-2</v>
       </c>
-      <c r="E55" s="74"/>
-      <c r="F55" s="74"/>
+      <c r="E55" s="99"/>
+      <c r="F55" s="99"/>
       <c r="G55" s="35">
         <v>0.1033</v>
       </c>
-      <c r="H55" s="74"/>
-      <c r="I55" s="74"/>
+      <c r="H55" s="99"/>
+      <c r="I55" s="99"/>
       <c r="J55" s="33">
         <v>0.1085</v>
       </c>
@@ -2897,21 +3039,21 @@
       <c r="S55" s="1"/>
     </row>
     <row r="56" spans="1:19" ht="15">
-      <c r="A56" s="70" t="s">
+      <c r="A56" s="84" t="s">
         <v>54</v>
       </c>
-      <c r="B56" s="68"/>
-      <c r="C56" s="68"/>
+      <c r="B56" s="96"/>
+      <c r="C56" s="96"/>
       <c r="D56" s="31">
         <v>3.26</v>
       </c>
-      <c r="E56" s="68"/>
-      <c r="F56" s="68"/>
+      <c r="E56" s="96"/>
+      <c r="F56" s="96"/>
       <c r="G56" s="31">
         <v>2.48</v>
       </c>
-      <c r="H56" s="68"/>
-      <c r="I56" s="68"/>
+      <c r="H56" s="96"/>
+      <c r="I56" s="96"/>
       <c r="J56" s="37">
         <v>2.5</v>
       </c>
@@ -2926,19 +3068,19 @@
       <c r="S56" s="1"/>
     </row>
     <row r="57" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A57" s="72"/>
-      <c r="B57" s="69"/>
-      <c r="C57" s="69"/>
+      <c r="A57" s="85"/>
+      <c r="B57" s="97"/>
+      <c r="C57" s="97"/>
       <c r="D57" s="32">
         <v>8.3199999999999996E-2</v>
       </c>
-      <c r="E57" s="69"/>
-      <c r="F57" s="69"/>
+      <c r="E57" s="97"/>
+      <c r="F57" s="97"/>
       <c r="G57" s="32">
         <v>8.9399999999999993E-2</v>
       </c>
-      <c r="H57" s="69"/>
-      <c r="I57" s="69"/>
+      <c r="H57" s="97"/>
+      <c r="I57" s="97"/>
       <c r="J57" s="30">
         <v>9.2999999999999999E-2</v>
       </c>
@@ -3311,7 +3453,7 @@
       <c r="S67" s="1"/>
     </row>
     <row r="68" spans="1:19" ht="24">
-      <c r="A68" s="70" t="s">
+      <c r="A68" s="84" t="s">
         <v>65</v>
       </c>
       <c r="B68" s="40" t="s">
@@ -3352,7 +3494,7 @@
       <c r="S68" s="1"/>
     </row>
     <row r="69" spans="1:19" ht="36">
-      <c r="A69" s="71"/>
+      <c r="A69" s="106"/>
       <c r="B69" s="41" t="s">
         <v>67</v>
       </c>
@@ -3391,7 +3533,7 @@
       <c r="S69" s="1"/>
     </row>
     <row r="70" spans="1:19" ht="36">
-      <c r="A70" s="71"/>
+      <c r="A70" s="106"/>
       <c r="B70" s="41" t="s">
         <v>68</v>
       </c>
@@ -3430,7 +3572,7 @@
       <c r="S70" s="1"/>
     </row>
     <row r="71" spans="1:19" ht="24">
-      <c r="A71" s="71"/>
+      <c r="A71" s="106"/>
       <c r="B71" s="41" t="s">
         <v>69</v>
       </c>
@@ -3469,7 +3611,7 @@
       <c r="S71" s="1"/>
     </row>
     <row r="72" spans="1:19" ht="24">
-      <c r="A72" s="71"/>
+      <c r="A72" s="106"/>
       <c r="B72" s="41" t="s">
         <v>70</v>
       </c>
@@ -3508,7 +3650,7 @@
       <c r="S72" s="1"/>
     </row>
     <row r="73" spans="1:19" ht="24">
-      <c r="A73" s="71"/>
+      <c r="A73" s="106"/>
       <c r="B73" s="41" t="s">
         <v>71</v>
       </c>
@@ -3547,7 +3689,7 @@
       <c r="S73" s="1"/>
     </row>
     <row r="74" spans="1:19" ht="24">
-      <c r="A74" s="71"/>
+      <c r="A74" s="106"/>
       <c r="B74" s="41" t="s">
         <v>72</v>
       </c>
@@ -3586,7 +3728,7 @@
       <c r="S74" s="1"/>
     </row>
     <row r="75" spans="1:19" ht="24">
-      <c r="A75" s="71"/>
+      <c r="A75" s="106"/>
       <c r="B75" s="41" t="s">
         <v>73</v>
       </c>
@@ -3625,7 +3767,7 @@
       <c r="S75" s="1"/>
     </row>
     <row r="76" spans="1:19" ht="24">
-      <c r="A76" s="71"/>
+      <c r="A76" s="106"/>
       <c r="B76" s="41" t="s">
         <v>74</v>
       </c>
@@ -3664,7 +3806,7 @@
       <c r="S76" s="1"/>
     </row>
     <row r="77" spans="1:19" ht="24">
-      <c r="A77" s="71"/>
+      <c r="A77" s="106"/>
       <c r="B77" s="41" t="s">
         <v>75</v>
       </c>
@@ -3703,7 +3845,7 @@
       <c r="S77" s="1"/>
     </row>
     <row r="78" spans="1:19" ht="24">
-      <c r="A78" s="71"/>
+      <c r="A78" s="106"/>
       <c r="B78" s="41" t="s">
         <v>76</v>
       </c>
@@ -3742,7 +3884,7 @@
       <c r="S78" s="1"/>
     </row>
     <row r="79" spans="1:19" ht="24">
-      <c r="A79" s="71"/>
+      <c r="A79" s="106"/>
       <c r="B79" s="41" t="s">
         <v>77</v>
       </c>
@@ -3781,7 +3923,7 @@
       <c r="S79" s="1"/>
     </row>
     <row r="80" spans="1:19" ht="24">
-      <c r="A80" s="71"/>
+      <c r="A80" s="106"/>
       <c r="B80" s="41" t="s">
         <v>78</v>
       </c>
@@ -3820,7 +3962,7 @@
       <c r="S80" s="1"/>
     </row>
     <row r="81" spans="1:19" ht="24">
-      <c r="A81" s="71"/>
+      <c r="A81" s="106"/>
       <c r="B81" s="41" t="s">
         <v>79</v>
       </c>
@@ -3859,7 +4001,7 @@
       <c r="S81" s="1"/>
     </row>
     <row r="82" spans="1:19" ht="24">
-      <c r="A82" s="71"/>
+      <c r="A82" s="106"/>
       <c r="B82" s="41" t="s">
         <v>80</v>
       </c>
@@ -3898,7 +4040,7 @@
       <c r="S82" s="1"/>
     </row>
     <row r="83" spans="1:19" ht="24">
-      <c r="A83" s="71"/>
+      <c r="A83" s="106"/>
       <c r="B83" s="41" t="s">
         <v>81</v>
       </c>
@@ -3937,7 +4079,7 @@
       <c r="S83" s="1"/>
     </row>
     <row r="84" spans="1:19" ht="24">
-      <c r="A84" s="71"/>
+      <c r="A84" s="106"/>
       <c r="B84" s="41" t="s">
         <v>82</v>
       </c>
@@ -3976,7 +4118,7 @@
       <c r="S84" s="1"/>
     </row>
     <row r="85" spans="1:19" ht="24">
-      <c r="A85" s="71"/>
+      <c r="A85" s="106"/>
       <c r="B85" s="42"/>
       <c r="C85" s="42"/>
       <c r="D85" s="41" t="s">
@@ -4007,7 +4149,7 @@
       <c r="S85" s="1"/>
     </row>
     <row r="86" spans="1:19" ht="24">
-      <c r="A86" s="71"/>
+      <c r="A86" s="106"/>
       <c r="B86" s="42"/>
       <c r="C86" s="42"/>
       <c r="D86" s="41" t="s">
@@ -4034,7 +4176,7 @@
       <c r="S86" s="1"/>
     </row>
     <row r="87" spans="1:19" ht="24">
-      <c r="A87" s="71"/>
+      <c r="A87" s="106"/>
       <c r="B87" s="42"/>
       <c r="C87" s="42"/>
       <c r="D87" s="41" t="s">
@@ -4061,7 +4203,7 @@
       <c r="S87" s="1"/>
     </row>
     <row r="88" spans="1:19" ht="24">
-      <c r="A88" s="71"/>
+      <c r="A88" s="106"/>
       <c r="B88" s="42"/>
       <c r="C88" s="42"/>
       <c r="D88" s="41" t="s">
@@ -4088,7 +4230,7 @@
       <c r="S88" s="1"/>
     </row>
     <row r="89" spans="1:19" ht="24">
-      <c r="A89" s="71"/>
+      <c r="A89" s="106"/>
       <c r="B89" s="42"/>
       <c r="C89" s="42"/>
       <c r="D89" s="41" t="s">
@@ -4115,7 +4257,7 @@
       <c r="S89" s="1"/>
     </row>
     <row r="90" spans="1:19" ht="24">
-      <c r="A90" s="71"/>
+      <c r="A90" s="106"/>
       <c r="B90" s="42"/>
       <c r="C90" s="42"/>
       <c r="D90" s="41" t="s">
@@ -4142,7 +4284,7 @@
       <c r="S90" s="1"/>
     </row>
     <row r="91" spans="1:19" ht="24">
-      <c r="A91" s="71"/>
+      <c r="A91" s="106"/>
       <c r="B91" s="42"/>
       <c r="C91" s="42"/>
       <c r="D91" s="41" t="s">
@@ -4169,7 +4311,7 @@
       <c r="S91" s="1"/>
     </row>
     <row r="92" spans="1:19" ht="24">
-      <c r="A92" s="71"/>
+      <c r="A92" s="106"/>
       <c r="B92" s="42"/>
       <c r="C92" s="42"/>
       <c r="D92" s="41" t="s">
@@ -4196,7 +4338,7 @@
       <c r="S92" s="1"/>
     </row>
     <row r="93" spans="1:19" ht="24">
-      <c r="A93" s="71"/>
+      <c r="A93" s="106"/>
       <c r="B93" s="42"/>
       <c r="C93" s="42"/>
       <c r="D93" s="41" t="s">
@@ -4223,7 +4365,7 @@
       <c r="S93" s="1"/>
     </row>
     <row r="94" spans="1:19" ht="15">
-      <c r="A94" s="71"/>
+      <c r="A94" s="106"/>
       <c r="B94" s="42"/>
       <c r="C94" s="42"/>
       <c r="D94" s="42"/>
@@ -4248,7 +4390,7 @@
       <c r="S94" s="1"/>
     </row>
     <row r="95" spans="1:19" ht="15.75" thickBot="1">
-      <c r="A95" s="72"/>
+      <c r="A95" s="85"/>
       <c r="B95" s="48"/>
       <c r="C95" s="48"/>
       <c r="D95" s="48"/>
@@ -4272,45 +4414,78 @@
     </row>
   </sheetData>
   <mergeCells count="133">
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="I56:I57"/>
+    <mergeCell ref="A68:A95"/>
+    <mergeCell ref="H54:H55"/>
+    <mergeCell ref="I54:I55"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="E56:E57"/>
+    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="H56:H57"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="J52:J53"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="J45:J46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="I43:I44"/>
+    <mergeCell ref="J39:J40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="I39:I40"/>
+    <mergeCell ref="J35:J36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="I35:I36"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="C30:C31"/>
@@ -4333,78 +4508,45 @@
     <mergeCell ref="D26:D27"/>
     <mergeCell ref="E26:E27"/>
     <mergeCell ref="F26:F27"/>
-    <mergeCell ref="J35:J36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="I43:I44"/>
-    <mergeCell ref="J39:J40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="I39:I40"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="J45:J46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="J52:J53"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="I56:I57"/>
-    <mergeCell ref="A68:A95"/>
-    <mergeCell ref="H54:H55"/>
-    <mergeCell ref="I54:I55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="E56:E57"/>
-    <mergeCell ref="F56:F57"/>
-    <mergeCell ref="H56:H57"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="119" orientation="portrait" r:id="rId1"/>
@@ -4413,10 +4555,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:T95"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -4444,79 +4587,73 @@
       </c>
     </row>
     <row r="2" spans="1:18" ht="14.25" thickTop="1" thickBot="1">
-      <c r="A2" s="4" t="s">
-        <v>10</v>
+      <c r="A2" s="70" t="s">
+        <v>113</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="10"/>
       <c r="D2" s="9"/>
     </row>
-    <row r="3" spans="1:18" ht="60.75" thickBot="1">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:18" ht="13.5" thickBot="1">
+      <c r="A3" s="70" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+    </row>
+    <row r="4" spans="1:18" ht="72.75" thickBot="1">
+      <c r="A4" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D4" s="14" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="13.5" thickBot="1">
-      <c r="A4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="1:18" ht="13.5" thickBot="1">
       <c r="A5" s="47" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
       <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:18" ht="13.5" thickBot="1">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="70" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="79"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="79"/>
+    </row>
+    <row r="7" spans="1:18" ht="13.5" thickBot="1">
+      <c r="A7" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="91"/>
-      <c r="C6" s="91"/>
-      <c r="D6" s="91"/>
-    </row>
-    <row r="7" spans="1:18" ht="13.5" thickBot="1">
-      <c r="A7" s="4" t="s">
+      <c r="B7" s="108"/>
+      <c r="C7" s="108"/>
+      <c r="D7" s="108"/>
+    </row>
+    <row r="8" spans="1:18" ht="13.5" thickBot="1">
+      <c r="A8" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="92"/>
-      <c r="C7" s="92"/>
-      <c r="D7" s="92"/>
-    </row>
-    <row r="8" spans="1:18" ht="13.5" thickBot="1">
-      <c r="A8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="20">
-        <v>551.05999999999995</v>
-      </c>
-      <c r="C8" s="20">
-        <v>480.93</v>
-      </c>
-      <c r="D8" s="20">
-        <v>480.32</v>
-      </c>
-      <c r="I8" s="63" t="s">
+      <c r="B8" s="109"/>
+      <c r="C8" s="109"/>
+      <c r="D8" s="109"/>
+      <c r="I8" s="119" t="s">
         <v>94</v>
       </c>
-      <c r="J8" s="63" t="s">
+      <c r="J8" s="119" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="63" t="s">
+      <c r="K8" s="119" t="s">
         <v>106</v>
       </c>
       <c r="L8" s="63" t="s">
@@ -4542,17 +4679,17 @@
       </c>
     </row>
     <row r="9" spans="1:18" ht="13.5" thickBot="1">
-      <c r="A9" s="4" t="s">
-        <v>26</v>
+      <c r="A9" s="70" t="s">
+        <v>25</v>
       </c>
       <c r="B9" s="22">
-        <v>570.03</v>
+        <v>550.67999999999995</v>
       </c>
       <c r="C9" s="22">
-        <v>514.30999999999995</v>
+        <v>387.03</v>
       </c>
       <c r="D9" s="22">
-        <v>528.1</v>
+        <v>321.94</v>
       </c>
       <c r="I9" s="63" t="s">
         <v>95</v>
@@ -4570,31 +4707,37 @@
         <v>3</v>
       </c>
       <c r="N9" s="64">
-        <v>551.05999999999995</v>
+        <v>550.67999999999995</v>
       </c>
       <c r="O9" s="64">
-        <f>N9+(2*(L9+M9))</f>
-        <v>561.05999999999995</v>
+        <f>ROUND(N9+(2*(L9+M9)),2)</f>
+        <v>560.67999999999995</v>
       </c>
       <c r="P9" s="65">
-        <f>O9+( (2*SUM(L9+M9)*(SUM(L9+M9)+1))/(K9-SUM(L9+M9)-1) )</f>
-        <v>561.72666666666657</v>
+        <f>ROUND(O9+( (2*SUM(L9+M9)*(SUM(L9+M9)+1))/(K9-SUM(L9+M9)-1) ), 2)</f>
+        <v>561.35</v>
       </c>
       <c r="Q9" s="64">
-        <f>N9+(L9*LN(K9))</f>
-        <v>560.18869638293563</v>
+        <f>ROUND(N9+(L9*LN(K9)),2)</f>
+        <v>559.80999999999995</v>
       </c>
       <c r="R9" s="64">
-        <v>570.03</v>
+        <v>569.65</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="13.5" thickBot="1">
       <c r="A10" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
+        <v>26</v>
+      </c>
+      <c r="B10" s="16">
+        <v>569.65</v>
+      </c>
+      <c r="C10" s="16">
+        <v>420.41</v>
+      </c>
+      <c r="D10" s="16">
+        <v>369.72</v>
+      </c>
       <c r="I10" s="63" t="s">
         <v>96</v>
       </c>
@@ -4611,27 +4754,27 @@
         <v>5</v>
       </c>
       <c r="N10" s="64">
-        <v>480.93</v>
+        <v>387.03</v>
       </c>
       <c r="O10" s="64">
-        <f t="shared" ref="O10:O11" si="0">N10+(2*(L10+M10))</f>
-        <v>498.93</v>
+        <f t="shared" ref="O10:O11" si="0">ROUND(N10+(2*(L10+M10)),2)</f>
+        <v>405.03</v>
       </c>
       <c r="P10" s="65">
-        <f>O10+( (2*SUM(L10+M10)*(SUM(L10+M10)+1))/(K10-SUM(L10+M10)-1) )</f>
-        <v>501.02302325581394</v>
+        <f t="shared" ref="P10:P11" si="1">ROUND(O10+( (2*SUM(L10+M10)*(SUM(L10+M10)+1))/(K10-SUM(L10+M10)-1) ), 2)</f>
+        <v>407.12</v>
       </c>
       <c r="Q10" s="64">
-        <f t="shared" ref="Q10:Q11" si="1">N10+(L10*LN(K10))</f>
-        <v>499.18739276587132</v>
+        <f t="shared" ref="Q10:Q11" si="2">ROUND(N10+(L10*LN(K10)),2)</f>
+        <v>405.29</v>
       </c>
       <c r="R10" s="64">
-        <v>514.30999999999995</v>
+        <v>420.41</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="13.5" thickBot="1">
-      <c r="A11" s="4" t="s">
-        <v>28</v>
+      <c r="A11" s="70" t="s">
+        <v>27</v>
       </c>
       <c r="B11" s="24"/>
       <c r="C11" s="24"/>
@@ -4652,27 +4795,27 @@
         <v>7</v>
       </c>
       <c r="N11" s="64">
-        <v>480.32</v>
+        <v>321.94</v>
       </c>
       <c r="O11" s="64">
         <f t="shared" si="0"/>
-        <v>506.32</v>
+        <v>347.94</v>
       </c>
       <c r="P11" s="65">
-        <f t="shared" ref="P11" si="2">O11+( (2*SUM(L11+M11)*(SUM(L11+M11)+1))/(K11-SUM(L11+M11)-1) )</f>
-        <v>510.75902439024389</v>
+        <f t="shared" si="1"/>
+        <v>352.38</v>
       </c>
       <c r="Q11" s="64">
-        <f t="shared" si="1"/>
-        <v>507.706089148807</v>
+        <f t="shared" si="2"/>
+        <v>349.33</v>
       </c>
       <c r="R11" s="64">
-        <v>528.1</v>
+        <v>369.72</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="13.5" thickBot="1">
-      <c r="A12" s="4" t="s">
-        <v>29</v>
+      <c r="A12" s="70" t="s">
+        <v>28</v>
       </c>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
@@ -4680,152 +4823,189 @@
     </row>
     <row r="13" spans="1:18" ht="13.5" thickBot="1">
       <c r="A13" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>31</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="75" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="75" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="121" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="13.5" thickBot="1">
+      <c r="A15" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="50">
-        <v>52.08</v>
-      </c>
-      <c r="C14" s="83"/>
-      <c r="D14" s="83"/>
-    </row>
-    <row r="15" spans="1:18" ht="13.5" thickBot="1">
-      <c r="A15" s="72"/>
       <c r="B15" s="51">
-        <v>6.1699999999999998E-2</v>
-      </c>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
+        <v>49.87</v>
+      </c>
+      <c r="C15" s="76"/>
+      <c r="D15" s="76"/>
+      <c r="I15" s="120"/>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="70" t="s">
+      <c r="A16" s="70"/>
+      <c r="B16" s="110">
+        <v>7.5600000000000001E-2</v>
+      </c>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="I16" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="13.5" thickBot="1">
+      <c r="A17" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="52">
-        <v>10.35</v>
-      </c>
-      <c r="C16" s="52">
-        <v>10.19</v>
-      </c>
-      <c r="D16" s="52">
-        <v>10.24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A17" s="72"/>
       <c r="B17" s="54">
-        <v>7.2800000000000004E-2</v>
+        <v>10.4</v>
       </c>
       <c r="C17" s="54">
-        <v>7.5499999999999998E-2</v>
+        <v>10.28</v>
       </c>
       <c r="D17" s="54">
-        <v>7.4099999999999999E-2</v>
+        <v>10.25</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="J17" s="64">
+        <f>550.68-387.03</f>
+        <v>163.64999999999998</v>
       </c>
       <c r="T17" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:20">
-      <c r="A18" s="70" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="83"/>
-      <c r="C18" s="83"/>
-      <c r="D18" s="83"/>
+      <c r="A18" s="70"/>
+      <c r="B18" s="111">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="C18" s="111">
+        <v>7.0800000000000002E-2</v>
+      </c>
+      <c r="D18" s="111">
+        <v>7.1300000000000002E-2</v>
+      </c>
+      <c r="I18" s="123" t="s">
+        <v>121</v>
+      </c>
+      <c r="J18" s="122">
+        <v>1.8E-37</v>
+      </c>
+      <c r="K18" s="122"/>
     </row>
     <row r="19" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A19" s="72"/>
-      <c r="B19" s="84"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="84"/>
+      <c r="A19" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="76"/>
+      <c r="C19" s="76">
+        <v>41.35</v>
+      </c>
+      <c r="D19" s="76">
+        <v>42.04</v>
+      </c>
     </row>
     <row r="20" spans="1:20">
-      <c r="A20" s="70" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="87"/>
-      <c r="C20" s="52">
-        <v>43.28</v>
-      </c>
-      <c r="D20" s="52">
-        <v>42.95</v>
+      <c r="A20" s="70"/>
+      <c r="B20" s="77"/>
+      <c r="C20" s="110">
+        <v>0.1055</v>
+      </c>
+      <c r="D20" s="110">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A21" s="72"/>
-      <c r="B21" s="88"/>
+      <c r="A21" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="78"/>
       <c r="C21" s="54">
-        <v>7.6399999999999996E-2</v>
-      </c>
-      <c r="D21" s="54">
-        <v>8.9099999999999999E-2</v>
+        <v>11.14</v>
+      </c>
+      <c r="D21" s="54"/>
+      <c r="I21" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="J21" s="64">
+        <f>387.03-321.94</f>
+        <v>65.089999999999975</v>
       </c>
       <c r="T21" s="8" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:20">
-      <c r="A22" s="70" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="83"/>
-      <c r="C22" s="50">
-        <v>15.69</v>
-      </c>
-      <c r="D22" s="83"/>
+      <c r="A22" s="70"/>
+      <c r="B22" s="75"/>
+      <c r="C22" s="112">
+        <v>0.28710000000000002</v>
+      </c>
+      <c r="D22" s="75"/>
+      <c r="I22" s="123" t="s">
+        <v>121</v>
+      </c>
+      <c r="J22" s="122">
+        <v>7.16E-16</v>
+      </c>
     </row>
     <row r="23" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A23" s="72"/>
-      <c r="B23" s="84"/>
+      <c r="A23" s="71" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="76"/>
       <c r="C23" s="51">
-        <v>3.03E-7</v>
-      </c>
-      <c r="D23" s="84"/>
+        <v>50.25</v>
+      </c>
+      <c r="D23" s="76">
+        <v>56.38</v>
+      </c>
     </row>
     <row r="24" spans="1:20">
-      <c r="A24" s="70" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="87"/>
-      <c r="C24" s="52">
-        <v>35.950000000000003</v>
-      </c>
-      <c r="D24" s="52">
-        <v>56.38</v>
-      </c>
+      <c r="A24" s="70"/>
+      <c r="B24" s="77"/>
+      <c r="C24" s="110">
+        <v>7.6000000000000003E-7</v>
+      </c>
+      <c r="D24" s="52"/>
     </row>
     <row r="25" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A25" s="72"/>
-      <c r="B25" s="88"/>
-      <c r="C25" s="54">
-        <v>0.37619999999999998</v>
-      </c>
+      <c r="A25" s="71" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="78"/>
+      <c r="C25" s="54"/>
       <c r="D25" s="54">
-        <v>1.0700000000000001E-7</v>
+        <v>10.19</v>
       </c>
     </row>
     <row r="26" spans="1:20">
-      <c r="A26" s="70" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="83"/>
-      <c r="C26" s="83"/>
-      <c r="D26" s="50">
-        <v>10.91</v>
+      <c r="A26" s="70"/>
+      <c r="B26" s="75"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="112">
+        <v>0.2414</v>
       </c>
       <c r="I26" s="67" t="s">
         <v>94</v>
@@ -4859,39 +5039,39 @@
       </c>
     </row>
     <row r="27" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A27" s="72"/>
-      <c r="B27" s="84"/>
-      <c r="C27" s="84"/>
+      <c r="A27" s="71" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="76"/>
+      <c r="C27" s="76"/>
       <c r="D27" s="51">
-        <v>0.33610000000000001</v>
-      </c>
-      <c r="I27" s="95" t="s">
+        <v>0.41</v>
+      </c>
+      <c r="I27" s="107" t="s">
         <v>111</v>
       </c>
-      <c r="J27" s="95"/>
-      <c r="K27" s="95"/>
-      <c r="L27" s="95"/>
-      <c r="M27" s="95"/>
-      <c r="N27" s="95"/>
-      <c r="O27" s="95"/>
-      <c r="P27" s="95"/>
-      <c r="Q27" s="95"/>
-      <c r="R27" s="95"/>
+      <c r="J27" s="107"/>
+      <c r="K27" s="107"/>
+      <c r="L27" s="107"/>
+      <c r="M27" s="107"/>
+      <c r="N27" s="107"/>
+      <c r="O27" s="107"/>
+      <c r="P27" s="107"/>
+      <c r="Q27" s="107"/>
+      <c r="R27" s="107"/>
     </row>
     <row r="28" spans="1:20">
-      <c r="A28" s="70" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="87"/>
-      <c r="C28" s="87"/>
-      <c r="D28" s="52">
-        <v>0.42299999999999999</v>
+      <c r="A28" s="70"/>
+      <c r="B28" s="77"/>
+      <c r="C28" s="77"/>
+      <c r="D28" s="110">
+        <v>1.9000000000000001E-7</v>
       </c>
       <c r="I28" s="67" t="s">
         <v>107</v>
       </c>
       <c r="J28" s="8">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K28" s="63">
         <v>90</v>
@@ -4903,36 +5083,38 @@
         <v>3</v>
       </c>
       <c r="N28" s="66">
-        <v>570.12099999999998</v>
+        <v>550.67999999999995</v>
       </c>
       <c r="O28" s="66">
         <f>N28+(2*(L28+M28))</f>
-        <v>580.12099999999998</v>
+        <v>560.67999999999995</v>
       </c>
       <c r="P28" s="66">
         <f>O28+( (2*SUM(L28+M28)*(SUM(L28+M28)+1))/(K28-SUM(L28+M28)-1) )</f>
-        <v>580.83528571428565</v>
+        <v>561.39428571428562</v>
       </c>
       <c r="Q28" s="66">
         <f>N28+(L28*LN(K28))</f>
-        <v>579.12061934066048</v>
-      </c>
-      <c r="R28" s="66">
-        <v>589.03700000000003</v>
+        <v>559.67961934066045</v>
+      </c>
+      <c r="R28" s="64">
+        <v>569.65</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A29" s="72"/>
-      <c r="B29" s="88"/>
-      <c r="C29" s="88"/>
+      <c r="A29" s="71" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="78"/>
+      <c r="C29" s="78"/>
       <c r="D29" s="54">
-        <v>7.5499999999999994E-8</v>
+        <v>0.72</v>
       </c>
       <c r="I29" s="67" t="s">
         <v>108</v>
       </c>
       <c r="J29" s="8">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K29" s="63">
         <v>90</v>
@@ -4944,38 +5126,36 @@
         <v>5</v>
       </c>
       <c r="N29" s="66">
-        <v>516.09199999999998</v>
+        <v>387.03</v>
       </c>
       <c r="O29" s="66">
         <f t="shared" ref="O29:O34" si="3">N29+(2*(L29+M29))</f>
-        <v>534.09199999999998</v>
+        <v>405.03</v>
       </c>
       <c r="P29" s="66">
         <f t="shared" ref="P29:P34" si="4">O29+( (2*SUM(L29+M29)*(SUM(L29+M29)+1))/(K29-SUM(L29+M29)-1) )</f>
-        <v>536.34199999999998</v>
+        <v>407.28</v>
       </c>
       <c r="Q29" s="66">
         <f t="shared" ref="Q29:Q34" si="5">N29+(L29*LN(K29))</f>
-        <v>534.0912386813211</v>
-      </c>
-      <c r="R29" s="66">
-        <v>549.423</v>
+        <v>405.02923868132103</v>
+      </c>
+      <c r="R29" s="64">
+        <v>420.41</v>
       </c>
     </row>
     <row r="30" spans="1:20">
-      <c r="A30" s="70" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="83"/>
-      <c r="C30" s="83"/>
-      <c r="D30" s="50">
-        <v>1.1499999999999999</v>
+      <c r="A30" s="70"/>
+      <c r="B30" s="75"/>
+      <c r="C30" s="75"/>
+      <c r="D30" s="112">
+        <v>4.4000000000000002E-7</v>
       </c>
       <c r="I30" s="67" t="s">
         <v>109</v>
       </c>
       <c r="J30" s="8">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K30" s="63">
         <v>90</v>
@@ -4987,57 +5167,59 @@
         <v>7</v>
       </c>
       <c r="N30" s="66">
-        <v>516.39400000000001</v>
+        <v>321.94</v>
       </c>
       <c r="O30" s="66">
         <f>N30+(2*(L30+M30))</f>
-        <v>542.39400000000001</v>
+        <v>347.94</v>
       </c>
       <c r="P30" s="66">
         <f t="shared" si="4"/>
-        <v>547.18347368421053</v>
+        <v>352.72947368421052</v>
       </c>
       <c r="Q30" s="66">
         <f t="shared" si="5"/>
-        <v>543.39285802198162</v>
-      </c>
-      <c r="R30" s="66">
-        <v>564.14099999999996</v>
+        <v>348.93885802198156</v>
+      </c>
+      <c r="R30" s="64">
+        <v>369.72</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="13.5" thickBot="1">
-      <c r="A31" s="72"/>
-      <c r="B31" s="84"/>
-      <c r="C31" s="84"/>
-      <c r="D31" s="51">
-        <v>8.6299999999999999E-8</v>
-      </c>
-      <c r="I31" s="95" t="s">
+      <c r="A31" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="76" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="76" t="s">
+        <v>31</v>
+      </c>
+      <c r="D31" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31" s="107" t="s">
         <v>112</v>
       </c>
-      <c r="J31" s="95"/>
-      <c r="K31" s="95"/>
-      <c r="L31" s="95"/>
-      <c r="M31" s="95"/>
-      <c r="N31" s="95"/>
-      <c r="O31" s="95"/>
-      <c r="P31" s="95"/>
-      <c r="Q31" s="95"/>
-      <c r="R31" s="95"/>
+      <c r="J31" s="107"/>
+      <c r="K31" s="107"/>
+      <c r="L31" s="107"/>
+      <c r="M31" s="107"/>
+      <c r="N31" s="107"/>
+      <c r="O31" s="107"/>
+      <c r="P31" s="107"/>
+      <c r="Q31" s="107"/>
+      <c r="R31" s="107"/>
     </row>
     <row r="32" spans="1:20" ht="13.5" thickBot="1">
       <c r="A32" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C32" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" s="28" t="s">
-        <v>31</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B32" s="28">
+        <v>0.24</v>
+      </c>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
       <c r="I32" s="67" t="s">
         <v>107</v>
       </c>
@@ -5073,18 +5255,12 @@
       </c>
     </row>
     <row r="33" spans="1:18">
-      <c r="A33" s="70" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33" s="31">
-        <v>0.25800000000000001</v>
-      </c>
-      <c r="C33" s="31">
-        <v>0.26900000000000002</v>
-      </c>
-      <c r="D33" s="31">
-        <v>0.26700000000000002</v>
-      </c>
+      <c r="A33" s="70"/>
+      <c r="B33" s="113">
+        <v>0.28620000000000001</v>
+      </c>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
       <c r="I33" s="67" t="s">
         <v>108</v>
       </c>
@@ -5120,15 +5296,17 @@
       </c>
     </row>
     <row r="34" spans="1:18" ht="13.5" thickBot="1">
-      <c r="A34" s="72"/>
+      <c r="A34" s="71" t="s">
+        <v>42</v>
+      </c>
       <c r="B34" s="32">
-        <v>0.2041</v>
+        <v>0.26</v>
       </c>
       <c r="C34" s="32">
-        <v>0.20169999999999999</v>
+        <v>0.26</v>
       </c>
       <c r="D34" s="32">
-        <v>0.1933</v>
+        <v>0.27</v>
       </c>
       <c r="I34" s="67" t="s">
         <v>109</v>
@@ -5165,254 +5343,298 @@
       </c>
     </row>
     <row r="35" spans="1:18">
-      <c r="A35" s="70" t="s">
-        <v>43</v>
-      </c>
-      <c r="B35" s="34">
-        <v>0.17899999999999999</v>
-      </c>
-      <c r="C35" s="73"/>
-      <c r="D35" s="73"/>
+      <c r="A35" s="70"/>
+      <c r="B35" s="114">
+        <v>0.20330000000000001</v>
+      </c>
+      <c r="C35" s="115">
+        <v>0.19389999999999999</v>
+      </c>
+      <c r="D35" s="115">
+        <v>0.19070000000000001</v>
+      </c>
     </row>
     <row r="36" spans="1:18" ht="13.5" thickBot="1">
-      <c r="A36" s="72"/>
-      <c r="B36" s="35">
-        <v>0.33729999999999999</v>
-      </c>
-      <c r="C36" s="74"/>
-      <c r="D36" s="74"/>
+      <c r="A36" s="71" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="35"/>
+      <c r="C36" s="73">
+        <v>0.24</v>
+      </c>
+      <c r="D36" s="73">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="37" spans="1:18">
-      <c r="A37" s="70" t="s">
-        <v>44</v>
-      </c>
+      <c r="A37" s="70"/>
       <c r="B37" s="68"/>
-      <c r="C37" s="68"/>
-      <c r="D37" s="68"/>
+      <c r="C37" s="116">
+        <v>0.2447</v>
+      </c>
+      <c r="D37" s="116">
+        <v>0.2571</v>
+      </c>
     </row>
     <row r="38" spans="1:18" ht="13.5" thickBot="1">
-      <c r="A38" s="72"/>
+      <c r="A38" s="71" t="s">
+        <v>45</v>
+      </c>
       <c r="B38" s="69"/>
-      <c r="C38" s="69"/>
+      <c r="C38" s="69">
+        <v>0.73</v>
+      </c>
       <c r="D38" s="69"/>
     </row>
     <row r="39" spans="1:18">
-      <c r="A39" s="70" t="s">
-        <v>45</v>
-      </c>
-      <c r="B39" s="73"/>
-      <c r="C39" s="34">
-        <v>1.2800000000000001E-7</v>
-      </c>
-      <c r="D39" s="73"/>
+      <c r="A39" s="70"/>
+      <c r="B39" s="72"/>
+      <c r="C39" s="114">
+        <v>0.40129999999999999</v>
+      </c>
+      <c r="D39" s="72"/>
     </row>
     <row r="40" spans="1:18" ht="13.5" thickBot="1">
-      <c r="A40" s="72"/>
-      <c r="B40" s="74"/>
+      <c r="A40" s="71" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="73"/>
       <c r="C40" s="59">
-        <v>0.73319999999999996</v>
-      </c>
-      <c r="D40" s="74"/>
+        <v>5.5999999999999999E-8</v>
+      </c>
+      <c r="D40" s="73">
+        <v>3.2000000000000002E-8</v>
+      </c>
     </row>
     <row r="41" spans="1:18">
-      <c r="A41" s="70" t="s">
-        <v>46</v>
-      </c>
+      <c r="A41" s="70"/>
       <c r="B41" s="68"/>
-      <c r="C41" s="31">
-        <v>0.253</v>
-      </c>
-      <c r="D41" s="31">
-        <v>0.19400000000000001</v>
+      <c r="C41" s="113">
+        <v>3.9247999999999998</v>
+      </c>
+      <c r="D41" s="113">
+        <v>4.6845999999999997</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="13.5" thickBot="1">
-      <c r="A42" s="72"/>
+      <c r="A42" s="71" t="s">
+        <v>48</v>
+      </c>
       <c r="B42" s="69"/>
-      <c r="C42" s="32">
-        <v>0.22439999999999999</v>
-      </c>
+      <c r="C42" s="32"/>
       <c r="D42" s="32">
-        <v>0.32129999999999997</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="43" spans="1:18">
-      <c r="A43" s="70" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" s="73"/>
-      <c r="C43" s="34">
-        <v>0.97099999999999997</v>
-      </c>
-      <c r="D43" s="79">
-        <v>2.0100000000000001E-8</v>
+      <c r="A43" s="70"/>
+      <c r="B43" s="72"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="117">
+        <v>0.30299999999999999</v>
       </c>
     </row>
     <row r="44" spans="1:18" ht="13.5" thickBot="1">
-      <c r="A44" s="72"/>
-      <c r="B44" s="74"/>
-      <c r="C44" s="35">
-        <v>0.41839999999999999</v>
-      </c>
-      <c r="D44" s="80"/>
+      <c r="A44" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="73"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="74">
+        <v>5.1E-8</v>
+      </c>
     </row>
     <row r="45" spans="1:18">
-      <c r="A45" s="70" t="s">
-        <v>48</v>
-      </c>
+      <c r="A45" s="70"/>
       <c r="B45" s="68"/>
       <c r="C45" s="68"/>
-      <c r="D45" s="31">
-        <v>1.04</v>
+      <c r="D45" s="113">
+        <v>1.7706999999999999</v>
       </c>
     </row>
     <row r="46" spans="1:18" ht="13.5" thickBot="1">
-      <c r="A46" s="72"/>
+      <c r="A46" s="71" t="s">
+        <v>50</v>
+      </c>
       <c r="B46" s="69"/>
       <c r="C46" s="69"/>
       <c r="D46" s="32">
-        <v>0.33750000000000002</v>
+        <v>7.4000000000000001E-8</v>
       </c>
     </row>
     <row r="47" spans="1:18">
-      <c r="A47" s="70" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47" s="73"/>
-      <c r="C47" s="73"/>
-      <c r="D47" s="34">
-        <v>3.4499999999999998E-8</v>
+      <c r="A47" s="70"/>
+      <c r="B47" s="72"/>
+      <c r="C47" s="72"/>
+      <c r="D47" s="114">
+        <v>3.1757</v>
       </c>
     </row>
     <row r="48" spans="1:18" ht="13.5" thickBot="1">
-      <c r="A48" s="72"/>
-      <c r="B48" s="74"/>
-      <c r="C48" s="74"/>
-      <c r="D48" s="59">
-        <v>2.2536</v>
+      <c r="A48" s="71" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="73" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" s="73" t="s">
+        <v>31</v>
+      </c>
+      <c r="D48" s="59" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="70" t="s">
-        <v>50</v>
-      </c>
-      <c r="B49" s="68"/>
-      <c r="C49" s="68"/>
+        <v>52</v>
+      </c>
+      <c r="B49" s="68">
+        <v>3.22</v>
+      </c>
+      <c r="C49" s="68">
+        <v>6.3E-2</v>
+      </c>
       <c r="D49" s="31">
-        <v>4.3200000000000003E-8</v>
+        <v>6.2E-2</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A50" s="72"/>
-      <c r="B50" s="69"/>
-      <c r="C50" s="69"/>
+      <c r="A50" s="71"/>
+      <c r="B50" s="118">
+        <v>8.4900000000000003E-2</v>
+      </c>
+      <c r="C50" s="118">
+        <v>9.4399999999999998E-2</v>
+      </c>
       <c r="D50" s="60">
-        <v>1.0998000000000001</v>
+        <v>9.5899999999999999E-2</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="13.5" thickBot="1">
       <c r="A51" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="B51" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C51" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="D51" s="28" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+        <v>55</v>
+      </c>
+      <c r="B51" s="28"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="28"/>
+    </row>
+    <row r="52" spans="1:4" ht="36">
       <c r="A52" s="70" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B52" s="31">
-        <v>3.34</v>
+        <v>1000</v>
       </c>
       <c r="C52" s="31">
-        <v>1.79</v>
+        <v>1000</v>
       </c>
       <c r="D52" s="31">
-        <v>1.78</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A53" s="72"/>
+      <c r="A53" s="71" t="s">
+        <v>114</v>
+      </c>
       <c r="B53" s="32">
-        <v>8.48E-2</v>
+        <v>2000</v>
       </c>
       <c r="C53" s="32">
-        <v>9.3899999999999997E-2</v>
+        <v>5000</v>
       </c>
       <c r="D53" s="32">
-        <v>0.106</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="70" t="s">
-        <v>53</v>
-      </c>
-      <c r="B54" s="73"/>
-      <c r="C54" s="73"/>
-      <c r="D54" s="73"/>
+        <v>115</v>
+      </c>
+      <c r="B54" s="72">
+        <v>2000</v>
+      </c>
+      <c r="C54" s="72">
+        <v>2000</v>
+      </c>
+      <c r="D54" s="72">
+        <v>5000</v>
+      </c>
     </row>
     <row r="55" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A55" s="72"/>
-      <c r="B55" s="74"/>
-      <c r="C55" s="74"/>
-      <c r="D55" s="74"/>
-    </row>
-    <row r="56" spans="1:4">
+      <c r="A55" s="71" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55" s="73">
+        <v>2000</v>
+      </c>
+      <c r="C55" s="73">
+        <v>2000</v>
+      </c>
+      <c r="D55" s="73">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="36">
       <c r="A56" s="70" t="s">
-        <v>54</v>
-      </c>
-      <c r="B56" s="68"/>
-      <c r="C56" s="68"/>
-      <c r="D56" s="68"/>
-    </row>
-    <row r="57" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A57" s="72"/>
-      <c r="B57" s="69"/>
-      <c r="C57" s="69"/>
-      <c r="D57" s="69"/>
-    </row>
-    <row r="58" spans="1:4" ht="13.5" thickBot="1">
+        <v>60</v>
+      </c>
+      <c r="B56" s="68">
+        <v>1000</v>
+      </c>
+      <c r="C56" s="68">
+        <v>1000</v>
+      </c>
+      <c r="D56" s="68">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="24.75" thickBot="1">
+      <c r="A57" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="B57" s="69">
+        <v>0.8</v>
+      </c>
+      <c r="C57" s="69">
+        <v>0.8</v>
+      </c>
+      <c r="D57" s="69">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="24.75" thickBot="1">
       <c r="A58" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="B58" s="16"/>
-      <c r="C58" s="16"/>
-      <c r="D58" s="16"/>
-    </row>
-    <row r="59" spans="1:4" ht="36.75" thickBot="1">
-      <c r="A59" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B59" s="20">
-        <v>1000</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="B58" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="C58" s="16">
+        <v>0.8</v>
+      </c>
+      <c r="D58" s="16">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="24.75" thickBot="1">
+      <c r="A59" s="70" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" s="20"/>
       <c r="C59" s="20">
-        <v>1000</v>
-      </c>
-      <c r="D59" s="20">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="36.75" thickBot="1">
-      <c r="A60" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B60" s="22">
-        <v>2000</v>
-      </c>
+        <v>5000</v>
+      </c>
+      <c r="D59" s="20"/>
+    </row>
+    <row r="60" spans="1:4" ht="24.75" thickBot="1">
+      <c r="A60" s="70" t="s">
+        <v>117</v>
+      </c>
+      <c r="B60" s="22"/>
       <c r="C60" s="22">
-        <v>5000</v>
-      </c>
-      <c r="D60" s="22">
-        <v>5000</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="D60" s="22"/>
     </row>
     <row r="61" spans="1:4" ht="36.75" thickBot="1">
       <c r="A61" s="4" t="s">
@@ -5501,7 +5723,7 @@
       <c r="D67" s="16"/>
     </row>
     <row r="68" spans="1:4" ht="24">
-      <c r="A68" s="70" t="s">
+      <c r="A68" s="84" t="s">
         <v>65</v>
       </c>
       <c r="B68" s="40" t="s">
@@ -5515,7 +5737,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="36">
-      <c r="A69" s="71"/>
+      <c r="A69" s="106"/>
       <c r="B69" s="41" t="s">
         <v>67</v>
       </c>
@@ -5527,7 +5749,7 @@
       </c>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="71"/>
+      <c r="A70" s="106"/>
       <c r="B70" s="41" t="s">
         <v>68</v>
       </c>
@@ -5539,7 +5761,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="24">
-      <c r="A71" s="71"/>
+      <c r="A71" s="106"/>
       <c r="B71" s="41" t="s">
         <v>69</v>
       </c>
@@ -5551,7 +5773,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" ht="24">
-      <c r="A72" s="71"/>
+      <c r="A72" s="106"/>
       <c r="B72" s="41" t="s">
         <v>70</v>
       </c>
@@ -5563,7 +5785,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="24">
-      <c r="A73" s="71"/>
+      <c r="A73" s="106"/>
       <c r="B73" s="41" t="s">
         <v>71</v>
       </c>
@@ -5575,7 +5797,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="24">
-      <c r="A74" s="71"/>
+      <c r="A74" s="106"/>
       <c r="B74" s="41" t="s">
         <v>72</v>
       </c>
@@ -5587,7 +5809,7 @@
       </c>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="71"/>
+      <c r="A75" s="106"/>
       <c r="B75" s="41" t="s">
         <v>73</v>
       </c>
@@ -5599,7 +5821,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="24">
-      <c r="A76" s="71"/>
+      <c r="A76" s="106"/>
       <c r="B76" s="41" t="s">
         <v>74</v>
       </c>
@@ -5611,7 +5833,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" ht="24">
-      <c r="A77" s="71"/>
+      <c r="A77" s="106"/>
       <c r="B77" s="41" t="s">
         <v>75</v>
       </c>
@@ -5623,7 +5845,7 @@
       </c>
     </row>
     <row r="78" spans="1:4" ht="24">
-      <c r="A78" s="71"/>
+      <c r="A78" s="106"/>
       <c r="B78" s="41" t="s">
         <v>76</v>
       </c>
@@ -5635,7 +5857,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" ht="24">
-      <c r="A79" s="71"/>
+      <c r="A79" s="106"/>
       <c r="B79" s="41" t="s">
         <v>77</v>
       </c>
@@ -5647,7 +5869,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="24">
-      <c r="A80" s="71"/>
+      <c r="A80" s="106"/>
       <c r="B80" s="41" t="s">
         <v>78</v>
       </c>
@@ -5659,7 +5881,7 @@
       </c>
     </row>
     <row r="81" spans="1:4" ht="24">
-      <c r="A81" s="71"/>
+      <c r="A81" s="106"/>
       <c r="B81" s="41" t="s">
         <v>79</v>
       </c>
@@ -5671,7 +5893,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="24">
-      <c r="A82" s="71"/>
+      <c r="A82" s="106"/>
       <c r="B82" s="41" t="s">
         <v>80</v>
       </c>
@@ -5683,7 +5905,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" ht="24">
-      <c r="A83" s="71"/>
+      <c r="A83" s="106"/>
       <c r="B83" s="41" t="s">
         <v>81</v>
       </c>
@@ -5695,7 +5917,7 @@
       </c>
     </row>
     <row r="84" spans="1:4" ht="24">
-      <c r="A84" s="71"/>
+      <c r="A84" s="106"/>
       <c r="B84" s="41" t="s">
         <v>82</v>
       </c>
@@ -5707,7 +5929,7 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="15">
-      <c r="A85" s="71"/>
+      <c r="A85" s="106"/>
       <c r="B85" s="42"/>
       <c r="C85" s="42"/>
       <c r="D85" s="41" t="s">
@@ -5715,142 +5937,83 @@
       </c>
     </row>
     <row r="86" spans="1:4" ht="15">
-      <c r="A86" s="71"/>
+      <c r="A86" s="106"/>
       <c r="B86" s="42"/>
       <c r="C86" s="42"/>
       <c r="D86" s="42"/>
     </row>
     <row r="87" spans="1:4" ht="15">
-      <c r="A87" s="71"/>
+      <c r="A87" s="106"/>
       <c r="B87" s="42"/>
       <c r="C87" s="42"/>
       <c r="D87" s="42"/>
     </row>
     <row r="88" spans="1:4" ht="15">
-      <c r="A88" s="71"/>
+      <c r="A88" s="106"/>
       <c r="B88" s="42"/>
       <c r="C88" s="42"/>
       <c r="D88" s="42"/>
     </row>
     <row r="89" spans="1:4" ht="15">
-      <c r="A89" s="71"/>
+      <c r="A89" s="106"/>
       <c r="B89" s="42"/>
       <c r="C89" s="42"/>
       <c r="D89" s="42"/>
     </row>
     <row r="90" spans="1:4" ht="15">
-      <c r="A90" s="71"/>
+      <c r="A90" s="106"/>
       <c r="B90" s="42"/>
       <c r="C90" s="42"/>
       <c r="D90" s="42"/>
     </row>
     <row r="91" spans="1:4" ht="15">
-      <c r="A91" s="71"/>
+      <c r="A91" s="106"/>
       <c r="B91" s="42"/>
       <c r="C91" s="42"/>
       <c r="D91" s="42"/>
     </row>
     <row r="92" spans="1:4" ht="15">
-      <c r="A92" s="71"/>
+      <c r="A92" s="106"/>
       <c r="B92" s="42"/>
       <c r="C92" s="42"/>
       <c r="D92" s="42"/>
     </row>
     <row r="93" spans="1:4" ht="15">
-      <c r="A93" s="71"/>
+      <c r="A93" s="106"/>
       <c r="B93" s="42"/>
       <c r="C93" s="42"/>
       <c r="D93" s="42"/>
     </row>
     <row r="94" spans="1:4" ht="15">
-      <c r="A94" s="71"/>
+      <c r="A94" s="106"/>
       <c r="B94" s="42"/>
       <c r="C94" s="42"/>
       <c r="D94" s="42"/>
     </row>
     <row r="95" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A95" s="72"/>
+      <c r="A95" s="85"/>
       <c r="B95" s="48"/>
       <c r="C95" s="48"/>
       <c r="D95" s="48"/>
     </row>
   </sheetData>
-  <mergeCells count="64">
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
+  <mergeCells count="3">
     <mergeCell ref="A68:A95"/>
     <mergeCell ref="I31:R31"/>
     <mergeCell ref="I27:R27"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="A47:A48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="119" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:O95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:O10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -5916,17 +6079,17 @@
       <c r="A6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="91"/>
-      <c r="C6" s="91"/>
-      <c r="D6" s="93"/>
+      <c r="B6" s="86"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="88"/>
     </row>
     <row r="7" spans="1:15" ht="13.5" thickBot="1">
       <c r="A7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="92"/>
-      <c r="C7" s="92"/>
-      <c r="D7" s="94"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="87"/>
+      <c r="D7" s="89"/>
       <c r="F7" s="63" t="s">
         <v>94</v>
       </c>
@@ -6127,25 +6290,25 @@
       </c>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="70" t="s">
+      <c r="A14" s="84" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="50">
         <v>54.62</v>
       </c>
-      <c r="C14" s="83"/>
-      <c r="D14" s="89"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="82"/>
     </row>
     <row r="15" spans="1:15" ht="13.5" thickBot="1">
-      <c r="A15" s="72"/>
+      <c r="A15" s="85"/>
       <c r="B15" s="51">
         <v>5.5500000000000001E-2</v>
       </c>
-      <c r="C15" s="84"/>
-      <c r="D15" s="90"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="83"/>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="70" t="s">
+      <c r="A16" s="84" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="52">
@@ -6159,7 +6322,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A17" s="72"/>
+      <c r="A17" s="85"/>
       <c r="B17" s="54">
         <v>7.0199999999999999E-2</v>
       </c>
@@ -6171,7 +6334,7 @@
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="70" t="s">
+      <c r="A18" s="84" t="s">
         <v>34</v>
       </c>
       <c r="B18" s="50">
@@ -6185,7 +6348,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A19" s="72"/>
+      <c r="A19" s="85"/>
       <c r="B19" s="51">
         <v>5.8299999999999998E-2</v>
       </c>
@@ -6197,10 +6360,10 @@
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="70" t="s">
+      <c r="A20" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="87"/>
+      <c r="B20" s="90"/>
       <c r="C20" s="52">
         <v>46.36</v>
       </c>
@@ -6209,8 +6372,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A21" s="72"/>
-      <c r="B21" s="88"/>
+      <c r="A21" s="85"/>
+      <c r="B21" s="91"/>
       <c r="C21" s="54">
         <v>6.88E-2</v>
       </c>
@@ -6219,28 +6382,28 @@
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="70" t="s">
+      <c r="A22" s="84" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="83"/>
+      <c r="B22" s="80"/>
       <c r="C22" s="50">
         <v>14.14</v>
       </c>
-      <c r="D22" s="89"/>
+      <c r="D22" s="82"/>
     </row>
     <row r="23" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A23" s="72"/>
-      <c r="B23" s="84"/>
+      <c r="A23" s="85"/>
+      <c r="B23" s="81"/>
       <c r="C23" s="51">
         <v>5.6700000000000003E-7</v>
       </c>
-      <c r="D23" s="90"/>
+      <c r="D23" s="83"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="70" t="s">
+      <c r="A24" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="87"/>
+      <c r="B24" s="90"/>
       <c r="C24" s="52">
         <v>42.59</v>
       </c>
@@ -6249,8 +6412,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A25" s="72"/>
-      <c r="B25" s="88"/>
+      <c r="A25" s="85"/>
+      <c r="B25" s="91"/>
       <c r="C25" s="54">
         <v>0.40789999999999998</v>
       </c>
@@ -6259,55 +6422,55 @@
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="70" t="s">
+      <c r="A26" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="83"/>
-      <c r="C26" s="83"/>
+      <c r="B26" s="80"/>
+      <c r="C26" s="80"/>
       <c r="D26" s="56">
         <v>15.71</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A27" s="72"/>
-      <c r="B27" s="84"/>
-      <c r="C27" s="84"/>
+      <c r="A27" s="85"/>
+      <c r="B27" s="81"/>
+      <c r="C27" s="81"/>
       <c r="D27" s="57">
         <v>1.2499999999999999E-7</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="70" t="s">
+      <c r="A28" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="87"/>
-      <c r="C28" s="87"/>
+      <c r="B28" s="90"/>
+      <c r="C28" s="90"/>
       <c r="D28" s="53">
         <v>3.65</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A29" s="72"/>
-      <c r="B29" s="88"/>
-      <c r="C29" s="88"/>
+      <c r="A29" s="85"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="91"/>
       <c r="D29" s="55">
         <v>1.4100000000000001E-7</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="70" t="s">
+      <c r="A30" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="83"/>
-      <c r="C30" s="83"/>
+      <c r="B30" s="80"/>
+      <c r="C30" s="80"/>
       <c r="D30" s="56">
         <v>1.75</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A31" s="72"/>
-      <c r="B31" s="84"/>
-      <c r="C31" s="84"/>
+      <c r="A31" s="85"/>
+      <c r="B31" s="81"/>
+      <c r="C31" s="81"/>
       <c r="D31" s="57">
         <v>1.01E-7</v>
       </c>
@@ -6327,7 +6490,7 @@
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="70" t="s">
+      <c r="A33" s="84" t="s">
         <v>42</v>
       </c>
       <c r="B33" s="31">
@@ -6341,7 +6504,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A34" s="72"/>
+      <c r="A34" s="85"/>
       <c r="B34" s="32">
         <v>0.20530000000000001</v>
       </c>
@@ -6353,25 +6516,25 @@
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="70" t="s">
+      <c r="A35" s="84" t="s">
         <v>43</v>
       </c>
       <c r="B35" s="34">
         <v>0.16500000000000001</v>
       </c>
-      <c r="C35" s="73"/>
-      <c r="D35" s="81"/>
+      <c r="C35" s="98"/>
+      <c r="D35" s="94"/>
     </row>
     <row r="36" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A36" s="72"/>
+      <c r="A36" s="85"/>
       <c r="B36" s="35">
         <v>0.32319999999999999</v>
       </c>
-      <c r="C36" s="74"/>
-      <c r="D36" s="82"/>
+      <c r="C36" s="99"/>
+      <c r="D36" s="95"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="70" t="s">
+      <c r="A37" s="84" t="s">
         <v>44</v>
       </c>
       <c r="B37" s="31">
@@ -6385,7 +6548,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A38" s="72"/>
+      <c r="A38" s="85"/>
       <c r="B38" s="32">
         <v>0.2281</v>
       </c>
@@ -6397,28 +6560,28 @@
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="70" t="s">
+      <c r="A39" s="84" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="73"/>
+      <c r="B39" s="98"/>
       <c r="C39" s="34">
         <v>5.4900000000000002E-8</v>
       </c>
-      <c r="D39" s="81"/>
+      <c r="D39" s="94"/>
     </row>
     <row r="40" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A40" s="72"/>
-      <c r="B40" s="74"/>
+      <c r="A40" s="85"/>
+      <c r="B40" s="99"/>
       <c r="C40" s="59">
         <v>0.97760000000000002</v>
       </c>
-      <c r="D40" s="82"/>
+      <c r="D40" s="95"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="70" t="s">
+      <c r="A41" s="84" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="68"/>
+      <c r="B41" s="96"/>
       <c r="C41" s="31">
         <v>0.216</v>
       </c>
@@ -6427,8 +6590,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A42" s="72"/>
-      <c r="B42" s="69"/>
+      <c r="A42" s="85"/>
+      <c r="B42" s="97"/>
       <c r="C42" s="32">
         <v>0.2843</v>
       </c>
@@ -6437,10 +6600,10 @@
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" s="70" t="s">
+      <c r="A43" s="84" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="73"/>
+      <c r="B43" s="98"/>
       <c r="C43" s="34">
         <v>1.05</v>
       </c>
@@ -6449,8 +6612,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A44" s="72"/>
-      <c r="B44" s="74"/>
+      <c r="A44" s="85"/>
+      <c r="B44" s="99"/>
       <c r="C44" s="35">
         <v>0.36849999999999999</v>
       </c>
@@ -6459,53 +6622,53 @@
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" s="70" t="s">
+      <c r="A45" s="84" t="s">
         <v>48</v>
       </c>
-      <c r="B45" s="68"/>
-      <c r="C45" s="68"/>
-      <c r="D45" s="77">
+      <c r="B45" s="96"/>
+      <c r="C45" s="96"/>
+      <c r="D45" s="102">
         <v>3.77E-8</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A46" s="72"/>
-      <c r="B46" s="69"/>
-      <c r="C46" s="69"/>
-      <c r="D46" s="78"/>
+      <c r="A46" s="85"/>
+      <c r="B46" s="97"/>
+      <c r="C46" s="97"/>
+      <c r="D46" s="103"/>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="70" t="s">
+      <c r="A47" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="B47" s="73"/>
-      <c r="C47" s="73"/>
+      <c r="B47" s="98"/>
+      <c r="C47" s="98"/>
       <c r="D47" s="36">
         <v>3.7100000000000001E-8</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A48" s="72"/>
-      <c r="B48" s="74"/>
-      <c r="C48" s="74"/>
+      <c r="A48" s="85"/>
+      <c r="B48" s="99"/>
+      <c r="C48" s="99"/>
       <c r="D48" s="62">
         <v>0.69159999999999999</v>
       </c>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="70" t="s">
+      <c r="A49" s="84" t="s">
         <v>50</v>
       </c>
-      <c r="B49" s="68"/>
-      <c r="C49" s="68"/>
+      <c r="B49" s="96"/>
+      <c r="C49" s="96"/>
       <c r="D49" s="37">
         <v>4.8100000000000001E-8</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A50" s="72"/>
-      <c r="B50" s="69"/>
-      <c r="C50" s="69"/>
+      <c r="A50" s="85"/>
+      <c r="B50" s="97"/>
+      <c r="C50" s="97"/>
       <c r="D50" s="61">
         <v>1.5687</v>
       </c>
@@ -6525,21 +6688,21 @@
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="70" t="s">
+      <c r="A52" s="84" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="68"/>
-      <c r="C52" s="68"/>
-      <c r="D52" s="75"/>
+      <c r="B52" s="96"/>
+      <c r="C52" s="96"/>
+      <c r="D52" s="104"/>
     </row>
     <row r="53" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A53" s="72"/>
-      <c r="B53" s="69"/>
-      <c r="C53" s="69"/>
-      <c r="D53" s="76"/>
+      <c r="A53" s="85"/>
+      <c r="B53" s="97"/>
+      <c r="C53" s="97"/>
+      <c r="D53" s="105"/>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="70" t="s">
+      <c r="A54" s="84" t="s">
         <v>53</v>
       </c>
       <c r="B54" s="34">
@@ -6553,7 +6716,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A55" s="72"/>
+      <c r="A55" s="85"/>
       <c r="B55" s="35">
         <v>8.4699999999999998E-2</v>
       </c>
@@ -6565,7 +6728,7 @@
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="70" t="s">
+      <c r="A56" s="84" t="s">
         <v>54</v>
       </c>
       <c r="B56" s="31">
@@ -6579,7 +6742,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="13.5" thickBot="1">
-      <c r="A57" s="72"/>
+      <c r="A57" s="85"/>
       <c r="B57" s="32">
         <v>8.3199999999999996E-2</v>
       </c>
@@ -6715,7 +6878,7 @@
       <c r="D67" s="17"/>
     </row>
     <row r="68" spans="1:4" ht="24">
-      <c r="A68" s="70" t="s">
+      <c r="A68" s="84" t="s">
         <v>65</v>
       </c>
       <c r="B68" s="40" t="s">
@@ -6729,7 +6892,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="36">
-      <c r="A69" s="71"/>
+      <c r="A69" s="106"/>
       <c r="B69" s="41" t="s">
         <v>67</v>
       </c>
@@ -6741,7 +6904,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="36">
-      <c r="A70" s="71"/>
+      <c r="A70" s="106"/>
       <c r="B70" s="41" t="s">
         <v>68</v>
       </c>
@@ -6753,7 +6916,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="24">
-      <c r="A71" s="71"/>
+      <c r="A71" s="106"/>
       <c r="B71" s="41" t="s">
         <v>69</v>
       </c>
@@ -6765,7 +6928,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" ht="24">
-      <c r="A72" s="71"/>
+      <c r="A72" s="106"/>
       <c r="B72" s="41" t="s">
         <v>70</v>
       </c>
@@ -6777,7 +6940,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="24">
-      <c r="A73" s="71"/>
+      <c r="A73" s="106"/>
       <c r="B73" s="41" t="s">
         <v>83</v>
       </c>
@@ -6789,7 +6952,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="24">
-      <c r="A74" s="71"/>
+      <c r="A74" s="106"/>
       <c r="B74" s="41" t="s">
         <v>84</v>
       </c>
@@ -6801,7 +6964,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="24">
-      <c r="A75" s="71"/>
+      <c r="A75" s="106"/>
       <c r="B75" s="41" t="s">
         <v>71</v>
       </c>
@@ -6813,7 +6976,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="24">
-      <c r="A76" s="71"/>
+      <c r="A76" s="106"/>
       <c r="B76" s="41" t="s">
         <v>72</v>
       </c>
@@ -6825,7 +6988,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" ht="24">
-      <c r="A77" s="71"/>
+      <c r="A77" s="106"/>
       <c r="B77" s="41" t="s">
         <v>73</v>
       </c>
@@ -6837,7 +7000,7 @@
       </c>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="71"/>
+      <c r="A78" s="106"/>
       <c r="B78" s="41" t="s">
         <v>85</v>
       </c>
@@ -6849,7 +7012,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" ht="24">
-      <c r="A79" s="71"/>
+      <c r="A79" s="106"/>
       <c r="B79" s="41" t="s">
         <v>74</v>
       </c>
@@ -6861,7 +7024,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="24">
-      <c r="A80" s="71"/>
+      <c r="A80" s="106"/>
       <c r="B80" s="41" t="s">
         <v>86</v>
       </c>
@@ -6873,7 +7036,7 @@
       </c>
     </row>
     <row r="81" spans="1:4" ht="24">
-      <c r="A81" s="71"/>
+      <c r="A81" s="106"/>
       <c r="B81" s="41" t="s">
         <v>75</v>
       </c>
@@ -6885,7 +7048,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="24">
-      <c r="A82" s="71"/>
+      <c r="A82" s="106"/>
       <c r="B82" s="41" t="s">
         <v>87</v>
       </c>
@@ -6897,7 +7060,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" ht="24">
-      <c r="A83" s="71"/>
+      <c r="A83" s="106"/>
       <c r="B83" s="41" t="s">
         <v>76</v>
       </c>
@@ -6909,7 +7072,7 @@
       </c>
     </row>
     <row r="84" spans="1:4" ht="24">
-      <c r="A84" s="71"/>
+      <c r="A84" s="106"/>
       <c r="B84" s="41" t="s">
         <v>77</v>
       </c>
@@ -6921,7 +7084,7 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="24">
-      <c r="A85" s="71"/>
+      <c r="A85" s="106"/>
       <c r="B85" s="41" t="s">
         <v>88</v>
       </c>
@@ -6933,7 +7096,7 @@
       </c>
     </row>
     <row r="86" spans="1:4" ht="24">
-      <c r="A86" s="71"/>
+      <c r="A86" s="106"/>
       <c r="B86" s="41" t="s">
         <v>78</v>
       </c>
@@ -6945,7 +7108,7 @@
       </c>
     </row>
     <row r="87" spans="1:4" ht="24">
-      <c r="A87" s="71"/>
+      <c r="A87" s="106"/>
       <c r="B87" s="41" t="s">
         <v>79</v>
       </c>
@@ -6957,7 +7120,7 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="24">
-      <c r="A88" s="71"/>
+      <c r="A88" s="106"/>
       <c r="B88" s="41" t="s">
         <v>89</v>
       </c>
@@ -6969,7 +7132,7 @@
       </c>
     </row>
     <row r="89" spans="1:4" ht="24">
-      <c r="A89" s="71"/>
+      <c r="A89" s="106"/>
       <c r="B89" s="41" t="s">
         <v>80</v>
       </c>
@@ -6981,7 +7144,7 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="24">
-      <c r="A90" s="71"/>
+      <c r="A90" s="106"/>
       <c r="B90" s="41" t="s">
         <v>90</v>
       </c>
@@ -6993,7 +7156,7 @@
       </c>
     </row>
     <row r="91" spans="1:4" ht="24">
-      <c r="A91" s="71"/>
+      <c r="A91" s="106"/>
       <c r="B91" s="41" t="s">
         <v>81</v>
       </c>
@@ -7005,7 +7168,7 @@
       </c>
     </row>
     <row r="92" spans="1:4" ht="24">
-      <c r="A92" s="71"/>
+      <c r="A92" s="106"/>
       <c r="B92" s="41" t="s">
         <v>82</v>
       </c>
@@ -7017,7 +7180,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" ht="24">
-      <c r="A93" s="71"/>
+      <c r="A93" s="106"/>
       <c r="B93" s="41" t="s">
         <v>91</v>
       </c>
@@ -7029,7 +7192,7 @@
       </c>
     </row>
     <row r="94" spans="1:4" ht="15">
-      <c r="A94" s="71"/>
+      <c r="A94" s="106"/>
       <c r="B94" s="42"/>
       <c r="C94" s="41" t="s">
         <v>91</v>
@@ -7039,7 +7202,7 @@
       </c>
     </row>
     <row r="95" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A95" s="72"/>
+      <c r="A95" s="85"/>
       <c r="B95" s="48"/>
       <c r="C95" s="48"/>
       <c r="D95" s="49" t="s">
@@ -7048,12 +7211,42 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="A68:A95"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
     <mergeCell ref="D52:D53"/>
     <mergeCell ref="A54:A55"/>
     <mergeCell ref="A49:A50"/>
@@ -7065,42 +7258,12 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="A45:A46"/>
     <mergeCell ref="B45:B46"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A68:A95"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="C52:C53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>